<commit_message>
working with bugs.  Detects faulse winnings
</commit_message>
<xml_diff>
--- a/homeworks/diagonal.xlsx
+++ b/homeworks/diagonal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\github\pirple_python\homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D910EA-F5EA-47A9-87EE-ED4B79D0C688}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CD0EFB-0C49-4573-AB7A-7B810C2555F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2F2857D-10CB-488A-9AA6-4C0F302D7A30}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{F2F2857D-10CB-488A-9AA6-4C0F302D7A30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="194">
   <si>
     <t>x+cols-1</t>
   </si>
@@ -613,6 +613,9 @@
   </si>
   <si>
     <t>B+1</t>
+  </si>
+  <si>
+    <t>[a][b]</t>
   </si>
 </sst>
 </file>
@@ -1094,20 +1097,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0543CC-5521-44C1-A1E5-9F2932D40B93}">
   <dimension ref="A2:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5100" topLeftCell="A48" activePane="bottomLeft"/>
-      <selection activeCell="H2" sqref="H2"/>
-      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="3744" topLeftCell="A74" activePane="bottomLeft"/>
+      <selection activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="H51" sqref="H51:P92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>5</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>4</v>
       </c>
@@ -1207,7 +1210,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>2</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>1</v>
       </c>
@@ -1357,7 +1360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>0</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B8" s="16">
         <v>0</v>
       </c>
@@ -1452,7 +1455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="N10" t="s">
         <v>35</v>
       </c>
@@ -1460,34 +1463,34 @@
         <v>1</v>
       </c>
       <c r="W10">
-        <f>V10+8</f>
+        <f t="shared" ref="W10:Y16" si="0">V10+8</f>
         <v>9</v>
       </c>
       <c r="X10">
-        <f>W10+8</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="Y10">
-        <f>X10+8</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="AA10">
         <v>1</v>
       </c>
       <c r="AB10">
-        <f>AA10+8</f>
+        <f t="shared" ref="AB10:AD18" si="1">AA10+8</f>
         <v>9</v>
       </c>
       <c r="AC10">
-        <f>AB10+8</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="AD10">
-        <f>AC10+8</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J11" t="s">
         <v>22</v>
       </c>
@@ -1495,34 +1498,34 @@
         <v>9</v>
       </c>
       <c r="W11">
-        <f>V11+8</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="X11">
-        <f>W11+8</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="Y11">
-        <f>X11+8</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="AA11">
         <v>2</v>
       </c>
       <c r="AB11">
-        <f>AA11+8</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AC11">
-        <f>AB11+8</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="AD11">
-        <f>AC11+8</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I12" s="18">
         <v>0</v>
       </c>
@@ -1550,40 +1553,40 @@
         <v>17</v>
       </c>
       <c r="W12">
-        <f>V12+8</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="X12">
-        <f>W12+8</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="Y12">
-        <f>X12+8</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="AA12">
         <v>3</v>
       </c>
       <c r="AB12">
-        <f>AA12+8</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="AC12">
-        <f>AB12+8</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="AD12">
-        <f>AC12+8</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I13" s="18">
-        <f>I12+1</f>
+        <f t="shared" ref="I13:J17" si="2">I12+1</f>
         <v>1</v>
       </c>
       <c r="J13">
-        <f>J12+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K13" t="s">
@@ -1596,7 +1599,7 @@
         <v>25</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13:O17" si="0">0+(8*J13)</f>
+        <f t="shared" ref="O13:O17" si="3">0+(8*J13)</f>
         <v>8</v>
       </c>
       <c r="Q13">
@@ -1606,43 +1609,43 @@
         <v>2</v>
       </c>
       <c r="W13">
-        <f>V13+8</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="X13">
-        <f>W13+8</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="Y13">
-        <f>X13+8</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="AA13">
         <v>4</v>
       </c>
       <c r="AB13">
-        <f>AA13+8</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="AC13">
-        <f>AB13+8</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AD13">
-        <f>AC13+8</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="18">
-        <f>I13+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J14">
-        <f>J13+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K14" t="s">
@@ -1655,7 +1658,7 @@
         <v>26</v>
       </c>
       <c r="O14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="Q14">
@@ -1665,40 +1668,40 @@
         <v>10</v>
       </c>
       <c r="W14">
-        <f>V14+8</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="X14">
-        <f>W14+8</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="Y14">
-        <f>X14+8</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="AA14">
         <v>9</v>
       </c>
       <c r="AB14">
-        <f>AA14+8</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="AC14">
-        <f>AB14+8</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="AD14">
-        <f>AC14+8</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I15" s="18">
-        <f>I14+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J15">
-        <f>J14+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K15" t="s">
@@ -1711,7 +1714,7 @@
         <v>27</v>
       </c>
       <c r="O15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="Q15">
@@ -1721,40 +1724,40 @@
         <v>18</v>
       </c>
       <c r="W15">
-        <f>V15+8</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="X15">
-        <f>W15+8</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="Y15">
-        <f>X15+8</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="AA15">
         <v>10</v>
       </c>
       <c r="AB15">
-        <f>AA15+8</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="AC15">
-        <f>AB15+8</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="AD15">
-        <f>AC15+8</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I16" s="18">
-        <f>I15+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J16">
-        <f>J15+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K16" t="s">
@@ -1767,7 +1770,7 @@
         <v>28</v>
       </c>
       <c r="O16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="Q16">
@@ -1777,40 +1780,40 @@
         <v>4</v>
       </c>
       <c r="W16">
-        <f>V16+8</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="X16">
-        <f>W16+8</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="Y16">
-        <f>X16+8</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="AA16">
         <v>11</v>
       </c>
       <c r="AB16">
-        <f>AA16+8</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="AC16">
-        <f>AB16+8</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="AD16">
-        <f>AC16+8</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
       <c r="I17" s="18">
-        <f>I16+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J17">
-        <f>J16+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K17" t="s">
@@ -1823,7 +1826,7 @@
         <v>29</v>
       </c>
       <c r="O17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="Q17">
@@ -1833,36 +1836,36 @@
         <v>17</v>
       </c>
       <c r="AB17">
-        <f>AA17+8</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="AC17">
-        <f>AB17+8</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="AD17">
-        <f>AC17+8</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="AA18">
         <v>18</v>
       </c>
       <c r="AB18">
-        <f>AA18+8</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="AC18">
-        <f>AB18+8</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="AD18">
-        <f>AC18+8</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="I19" s="18">
         <v>0</v>
       </c>
@@ -1887,13 +1890,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
       <c r="I20" s="18">
-        <f>I19+1</f>
+        <f t="shared" ref="I20:J24" si="4">I19+1</f>
         <v>1</v>
       </c>
       <c r="J20">
-        <f>J19+1</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K20" t="s">
@@ -1906,20 +1909,20 @@
         <v>24</v>
       </c>
       <c r="O20">
-        <f t="shared" ref="O20:O24" si="1">1+(8*I20)</f>
+        <f t="shared" ref="O20:O24" si="5">1+(8*I20)</f>
         <v>9</v>
       </c>
       <c r="Q20">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="I21" s="18">
-        <f>I20+1</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J21">
-        <f>J20+1</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="K21" t="s">
@@ -1932,20 +1935,20 @@
         <v>31</v>
       </c>
       <c r="O21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="Q21">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
       <c r="I22" s="18">
-        <f>I21+1</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="J22">
-        <f>J21+1</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="K22" t="s">
@@ -1958,35 +1961,35 @@
         <v>32</v>
       </c>
       <c r="O22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="Q22">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>15</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:E25" si="2">B23+8</f>
+        <f t="shared" ref="C23:E25" si="6">B23+8</f>
         <v>23</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="E23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="I23" s="18">
-        <f>I22+1</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="J23">
-        <f>J22+1</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="K23" t="s">
@@ -1999,27 +2002,27 @@
         <v>33</v>
       </c>
       <c r="O23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="Q23">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>8</v>
       </c>
       <c r="C24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="E24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="F24">
@@ -2027,11 +2030,11 @@
         <v>40</v>
       </c>
       <c r="I24" s="18">
-        <f>I23+1</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="J24">
-        <f>J23+1</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K24" t="s">
@@ -2044,27 +2047,27 @@
         <v>34</v>
       </c>
       <c r="O24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="Q24">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="F25" s="2">
@@ -2076,7 +2079,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
         <v>2</v>
       </c>
@@ -2085,19 +2088,19 @@
         <v>10</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" ref="D26:G26" si="3">C26+8</f>
+        <f t="shared" ref="D26:G26" si="7">C26+8</f>
         <v>18</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
       <c r="I26" s="18">
@@ -2120,7 +2123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
         <v>3</v>
       </c>
@@ -2129,24 +2132,24 @@
         <v>11</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" ref="D27:F27" si="4">C27+8</f>
+        <f t="shared" ref="D27:F27" si="8">C27+8</f>
         <v>19</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
       <c r="G27" s="2"/>
       <c r="I27" s="18">
-        <f>I26+1</f>
+        <f t="shared" ref="I27:J30" si="9">I26+1</f>
         <v>1</v>
       </c>
       <c r="J27">
-        <f>J26+1</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="K27" t="s">
@@ -2156,14 +2159,14 @@
         <v>10</v>
       </c>
       <c r="O27">
-        <f t="shared" ref="O27:O30" si="5">2+(8*I27)</f>
+        <f t="shared" ref="O27:O30" si="10">2+(8*I27)</f>
         <v>10</v>
       </c>
       <c r="Q27">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>4</v>
       </c>
@@ -2172,21 +2175,21 @@
         <v>12</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" ref="D28:E28" si="6">C28+8</f>
+        <f t="shared" ref="D28:E28" si="11">C28+8</f>
         <v>20</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>28</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="I28" s="18">
-        <f>I27+1</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="J28">
-        <f>J27+1</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K28" t="s">
@@ -2196,20 +2199,20 @@
         <v>18</v>
       </c>
       <c r="O28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="Q28">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="I29" s="18">
-        <f>I28+1</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="J29">
-        <f>J28+1</f>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="K29" t="s">
@@ -2219,20 +2222,20 @@
         <v>26</v>
       </c>
       <c r="O29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>26</v>
       </c>
       <c r="Q29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="I30" s="18">
-        <f>I29+1</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="J30">
-        <f>J29+1</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="K30" t="s">
@@ -2242,14 +2245,14 @@
         <v>34</v>
       </c>
       <c r="O30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>34</v>
       </c>
       <c r="Q30">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
       <c r="I32" s="18">
         <v>0</v>
       </c>
@@ -2270,13 +2273,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I33" s="18">
-        <f>I32+1</f>
+        <f t="shared" ref="I33:J35" si="12">I32+1</f>
         <v>1</v>
       </c>
       <c r="J33">
-        <f>J32+1</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="K33" t="s">
@@ -2286,20 +2289,20 @@
         <v>11</v>
       </c>
       <c r="O33">
-        <f t="shared" ref="O33:O35" si="7">3+(8*I33)</f>
+        <f t="shared" ref="O33:O35" si="13">3+(8*I33)</f>
         <v>11</v>
       </c>
       <c r="Q33">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I34" s="18">
-        <f>I33+1</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="J34">
-        <f>J33+1</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="K34" t="s">
@@ -2309,20 +2312,20 @@
         <v>19</v>
       </c>
       <c r="O34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="Q34">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I35" s="18">
-        <f>I34+1</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="J35">
-        <f>J34+1</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="K35" t="s">
@@ -2332,14 +2335,14 @@
         <v>27</v>
       </c>
       <c r="O35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="Q35">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2347,7 +2350,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2355,7 +2358,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D43" s="1">
         <v>0</v>
       </c>
@@ -2371,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D44" s="20">
         <v>0</v>
       </c>
@@ -2379,7 +2382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D45" s="5">
         <v>0</v>
       </c>
@@ -2387,7 +2390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D46" s="6">
         <v>0</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D47">
         <v>0</v>
       </c>
@@ -2403,7 +2406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D48">
         <v>0</v>
       </c>
@@ -2411,7 +2414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D49">
         <v>0</v>
       </c>
@@ -2419,10 +2422,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D50" s="19"/>
     </row>
-    <row r="51" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D51" s="3">
         <v>1</v>
       </c>
@@ -2460,7 +2463,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="52" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D52" s="1">
         <v>1</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D53" s="4">
         <v>1</v>
       </c>
@@ -2530,7 +2533,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D54" s="5">
         <v>1</v>
       </c>
@@ -2562,7 +2565,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D55" s="6">
         <v>1</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="56" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D56" s="19">
         <v>1</v>
       </c>
@@ -2632,7 +2635,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="57" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D57" s="19">
         <v>1</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="58" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:23" x14ac:dyDescent="0.3">
       <c r="H58">
         <v>1</v>
       </c>
@@ -2698,8 +2701,11 @@
       <c r="V58" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="59" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="W58" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D59" s="2">
         <v>2</v>
       </c>
@@ -2734,7 +2740,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D60" s="3">
         <v>2</v>
       </c>
@@ -2769,7 +2775,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D61" s="1">
         <v>2</v>
       </c>
@@ -2804,7 +2810,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="62" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D62" s="4">
         <v>2</v>
       </c>
@@ -2839,7 +2845,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D63" s="5">
         <v>2</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D64" s="6">
         <v>2</v>
       </c>
@@ -2909,7 +2915,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="65" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D65">
         <v>2</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:23" x14ac:dyDescent="0.3">
       <c r="I66" s="22" t="s">
         <v>104</v>
       </c>
@@ -2976,7 +2982,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D67">
         <v>3</v>
       </c>
@@ -3011,7 +3017,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D68" s="2">
         <v>3</v>
       </c>
@@ -3046,7 +3052,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D69" s="3">
         <v>3</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D70" s="1">
         <v>3</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D71" s="4">
         <v>3</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="72" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D72" s="5">
         <v>3</v>
       </c>
@@ -3189,7 +3195,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D73" s="6">
         <v>3</v>
       </c>
@@ -3224,7 +3230,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="74" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:23" x14ac:dyDescent="0.3">
       <c r="I74" s="22" t="s">
         <v>105</v>
       </c>
@@ -3253,7 +3259,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D75">
         <v>4</v>
       </c>
@@ -3288,7 +3294,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D76">
         <v>4</v>
       </c>
@@ -3323,7 +3329,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="77" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D77" s="2">
         <v>4</v>
       </c>
@@ -3358,7 +3364,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="78" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D78" s="3">
         <v>4</v>
       </c>
@@ -3393,7 +3399,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="79" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D79" s="1">
         <v>4</v>
       </c>
@@ -3431,7 +3437,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D80" s="4">
         <v>4</v>
       </c>
@@ -3463,7 +3469,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D81" s="5">
         <v>4</v>
       </c>
@@ -3498,7 +3504,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="82" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:23" x14ac:dyDescent="0.3">
       <c r="I82" s="22" t="s">
         <v>106</v>
       </c>
@@ -3527,7 +3533,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="83" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D83">
         <v>5</v>
       </c>
@@ -3562,7 +3568,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="84" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D84">
         <v>5</v>
       </c>
@@ -3597,7 +3603,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="85" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D85">
         <v>5</v>
       </c>
@@ -3632,7 +3638,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="86" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D86" s="2">
         <v>5</v>
       </c>
@@ -3670,7 +3676,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="87" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D87" s="3">
         <v>5</v>
       </c>
@@ -3705,7 +3711,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="88" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D88" s="1">
         <v>5</v>
       </c>
@@ -3740,7 +3746,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:23" x14ac:dyDescent="0.3">
       <c r="D89" s="4">
         <v>5</v>
       </c>
@@ -3775,7 +3781,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="90" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:23" x14ac:dyDescent="0.3">
       <c r="I90" s="22" t="s">
         <v>107</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="91" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:23" x14ac:dyDescent="0.3">
       <c r="I91" s="22" t="s">
         <v>47</v>
       </c>
@@ -3833,7 +3839,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="92" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:23" x14ac:dyDescent="0.3">
       <c r="I92" s="22" t="s">
         <v>53</v>
       </c>
@@ -3862,32 +3868,32 @@
         <v>179</v>
       </c>
     </row>
-    <row r="93" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:23" x14ac:dyDescent="0.3">
       <c r="W93" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="94" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:23" x14ac:dyDescent="0.3">
       <c r="W94" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="95" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:23" x14ac:dyDescent="0.3">
       <c r="W95" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:23" x14ac:dyDescent="0.3">
       <c r="W96" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="21:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="21:23" x14ac:dyDescent="0.3">
       <c r="W97" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="98" spans="21:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="21:23" x14ac:dyDescent="0.3">
       <c r="U98" t="s">
         <v>181</v>
       </c>
@@ -3895,7 +3901,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="21:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="21:23" x14ac:dyDescent="0.3">
       <c r="V99" t="s">
         <v>188</v>
       </c>

</xml_diff>